<commit_message>
updated calendar test summaries
</commit_message>
<xml_diff>
--- a/Nissan/Calendar_Processed_Data.xlsx
+++ b/Nissan/Calendar_Processed_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucsdcloud-my.sharepoint.com/personal/anaseri_ucsd_edu/Documents/college/research/Dr Tong ESS/Nissan cycle testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_0C36484E2FF259BAF6FF1CAB77FD6B56E3F4A67E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0B2D1AC-019A-4F85-B336-B3EA968ECF17}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_82B27C9B707F8ACEB29169FF9B41010EA5704278" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E9B6CC4-6FF5-4514-B155-13F623047E1B}"/>
   <bookViews>
-    <workbookView xWindow="-27240" yWindow="11490" windowWidth="25845" windowHeight="11325" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NP7" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="26">
   <si>
     <t>Test</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Characterization 4</t>
+  </si>
+  <si>
+    <t>Characterization 5</t>
   </si>
 </sst>
 </file>
@@ -107,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -124,6 +127,12 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -205,7 +214,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -525,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -540,67 +549,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -608,7 +617,7 @@
       <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="5">
         <v>44231</v>
       </c>
       <c r="C2">
@@ -673,7 +682,7 @@
       <c r="A3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>44372</v>
       </c>
       <c r="C3">
@@ -738,7 +747,7 @@
       <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="5">
         <v>44540.560972222222</v>
       </c>
       <c r="C4">
@@ -800,19 +809,82 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="5">
+        <v>44632.534074074072</v>
+      </c>
+      <c r="C5">
+        <v>90</v>
+      </c>
+      <c r="D5">
+        <v>76.568138888108152</v>
+      </c>
+      <c r="E5">
+        <v>62.403513893827913</v>
+      </c>
+      <c r="F5">
+        <v>33.544199138240053</v>
+      </c>
+      <c r="G5">
+        <v>33.692238932844248</v>
+      </c>
+      <c r="H5">
+        <v>33.719463233643111</v>
+      </c>
+      <c r="I5">
+        <v>33.781834685855159</v>
+      </c>
+      <c r="J5">
+        <v>33.335859643155523</v>
+      </c>
+      <c r="K5">
+        <v>33.301905457355367</v>
+      </c>
+      <c r="L5">
+        <v>33.350547337967477</v>
+      </c>
+      <c r="M5">
+        <v>33.287301617454347</v>
+      </c>
+      <c r="N5">
+        <v>33.377082734273181</v>
+      </c>
+      <c r="O5">
+        <v>33.293900189859507</v>
+      </c>
+      <c r="P5">
+        <v>33.166010594487453</v>
+      </c>
+      <c r="Q5">
+        <v>33.366218007052048</v>
+      </c>
+      <c r="R5">
+        <v>33.297953580330223</v>
+      </c>
+      <c r="S5">
+        <v>33.189980783355047</v>
+      </c>
+      <c r="T5">
+        <v>33.220561596040341</v>
+      </c>
+      <c r="U5">
+        <v>33.25777491657837</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A5" sqref="A5:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1150,6 +1222,71 @@
         <v>35.109798619837072</v>
       </c>
     </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3">
+        <v>44634.642418981479</v>
+      </c>
+      <c r="C6">
+        <v>92</v>
+      </c>
+      <c r="D6">
+        <v>73.851958333367818</v>
+      </c>
+      <c r="E6">
+        <v>67.317569435760632</v>
+      </c>
+      <c r="F6">
+        <v>34.859761132340367</v>
+      </c>
+      <c r="G6">
+        <v>34.850486558734517</v>
+      </c>
+      <c r="H6">
+        <v>34.776608365398488</v>
+      </c>
+      <c r="I6">
+        <v>34.845370118237227</v>
+      </c>
+      <c r="J6">
+        <v>34.654068191575043</v>
+      </c>
+      <c r="K6">
+        <v>34.731756989693189</v>
+      </c>
+      <c r="L6">
+        <v>34.535463097694013</v>
+      </c>
+      <c r="M6">
+        <v>34.740746517886748</v>
+      </c>
+      <c r="N6">
+        <v>34.904764233481757</v>
+      </c>
+      <c r="O6">
+        <v>34.815703860476432</v>
+      </c>
+      <c r="P6">
+        <v>34.559715414891251</v>
+      </c>
+      <c r="Q6">
+        <v>34.599788136387858</v>
+      </c>
+      <c r="R6">
+        <v>34.773796047071762</v>
+      </c>
+      <c r="S6">
+        <v>34.847453115741992</v>
+      </c>
+      <c r="T6">
+        <v>34.73648194407567</v>
+      </c>
+      <c r="U6">
+        <v>34.868794790944563</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -1158,10 +1295,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1173,67 +1310,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1430,6 +1567,71 @@
       </c>
       <c r="U4">
         <v>34.42087898913006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3">
+        <v>44635.736493055563</v>
+      </c>
+      <c r="C5">
+        <v>89</v>
+      </c>
+      <c r="D5">
+        <v>74.973930556947735</v>
+      </c>
+      <c r="E5">
+        <v>64.554263882706479</v>
+      </c>
+      <c r="F5">
+        <v>33.72963309975664</v>
+      </c>
+      <c r="G5">
+        <v>33.789970326062132</v>
+      </c>
+      <c r="H5">
+        <v>33.508187027161163</v>
+      </c>
+      <c r="I5">
+        <v>33.474074991272133</v>
+      </c>
+      <c r="J5">
+        <v>33.373986554002038</v>
+      </c>
+      <c r="K5">
+        <v>33.400366090564837</v>
+      </c>
+      <c r="L5">
+        <v>33.600651127523307</v>
+      </c>
+      <c r="M5">
+        <v>33.808582210134503</v>
+      </c>
+      <c r="N5">
+        <v>33.838498109488043</v>
+      </c>
+      <c r="O5">
+        <v>33.81863760412984</v>
+      </c>
+      <c r="P5">
+        <v>33.41863357577467</v>
+      </c>
+      <c r="Q5">
+        <v>33.511881602766231</v>
+      </c>
+      <c r="R5">
+        <v>33.361268707474167</v>
+      </c>
+      <c r="S5">
+        <v>33.453225569354252</v>
+      </c>
+      <c r="T5">
+        <v>33.959271862281938</v>
+      </c>
+      <c r="U5">
+        <v>34.037975455419407</v>
       </c>
     </row>
   </sheetData>
@@ -1439,10 +1641,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1456,67 +1658,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1524,7 +1726,7 @@
       <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="3">
         <v>44242</v>
       </c>
       <c r="C2">
@@ -1589,7 +1791,7 @@
       <c r="A3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="3">
         <v>44361</v>
       </c>
       <c r="C3">
@@ -1654,7 +1856,7 @@
       <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>44449.484594907408</v>
       </c>
       <c r="C4">
@@ -1719,7 +1921,7 @@
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>44571.69734953704</v>
       </c>
       <c r="C5">
@@ -1781,7 +1983,78 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3">
+        <v>44693.712314814817</v>
+      </c>
+      <c r="C6">
+        <v>121</v>
+      </c>
+      <c r="D6">
+        <v>59.507833333940461</v>
+      </c>
+      <c r="E6">
+        <v>61.349763896794421</v>
+      </c>
+      <c r="F6">
+        <v>33.29188262951574</v>
+      </c>
+      <c r="G6">
+        <v>33.287664182906681</v>
+      </c>
+      <c r="H6">
+        <v>32.959601620195443</v>
+      </c>
+      <c r="I6">
+        <v>33.069332169372373</v>
+      </c>
+      <c r="J6">
+        <v>33.04613960809727</v>
+      </c>
+      <c r="K6">
+        <v>33.174419727524857</v>
+      </c>
+      <c r="L6">
+        <v>33.331378782758897</v>
+      </c>
+      <c r="M6">
+        <v>33.277813162360403</v>
+      </c>
+      <c r="N6">
+        <v>33.550952700249319</v>
+      </c>
+      <c r="O6">
+        <v>33.588917030447327</v>
+      </c>
+      <c r="P6">
+        <v>33.121860651817059</v>
+      </c>
+      <c r="Q6">
+        <v>33.047985931617539</v>
+      </c>
+      <c r="R6">
+        <v>33.151182643107497</v>
+      </c>
+      <c r="S6">
+        <v>33.166388116514618</v>
+      </c>
+      <c r="T6">
+        <v>33.358733468632337</v>
+      </c>
+      <c r="U6">
+        <v>33.273162828941317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>